<commit_message>
Org doc and gannt chart done
</commit_message>
<xml_diff>
--- a/docs/Gantt Chart.xlsx
+++ b/docs/Gantt Chart.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3E1B706-D9F0-4FC4-ABEC-975CE7AA2AA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="29" documentId="13_ncr:1_{E3E1B706-D9F0-4FC4-ABEC-975CE7AA2AA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{03805296-5025-43C3-8A1A-7AA4E2BDCD25}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectSchedule" sheetId="11" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="56">
   <si>
     <t>Task 3</t>
   </si>
@@ -70,9 +70,6 @@
 TO</t>
   </si>
   <si>
-    <t>PROJECT TITLE</t>
-  </si>
-  <si>
     <t>Project Management Templates</t>
   </si>
   <si>
@@ -125,9 +122,6 @@
   </si>
   <si>
     <t>Click on the link below to visit vertex42.com and learn more about how to use this template, such as how to calculate days and work days, create task dependencies, change the colors of the bars, add a scroll bar to make it easier to change the display week, extend the date range displayed in the chart, etc.</t>
-  </si>
-  <si>
-    <t>Project Lead</t>
   </si>
   <si>
     <t>There are 2 worksheets in this workbook. 
@@ -145,9 +139,6 @@
   </si>
   <si>
     <t>date</t>
-  </si>
-  <si>
-    <t>Name</t>
   </si>
   <si>
     <t>Sample phase title block</t>
@@ -233,6 +224,30 @@
   </si>
   <si>
     <t>Sprint 4</t>
+  </si>
+  <si>
+    <t>Coding</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>Tech Doc</t>
+  </si>
+  <si>
+    <t>Org Doc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Presntation </t>
+  </si>
+  <si>
+    <t>Complexity Analyzer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aaron Downing </t>
+  </si>
+  <si>
+    <t>Ryerson Brower</t>
   </si>
 </sst>
 </file>
@@ -655,7 +670,7 @@
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -920,6 +935,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="8" applyBorder="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Comma" xfId="4" builtinId="3" customBuiltin="1"/>
@@ -1220,6 +1236,10 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1490,29 +1510,29 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
+      <selection pane="bottomLeft" activeCell="C3" sqref="C3:D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" style="58" customWidth="1"/>
-    <col min="2" max="2" width="19.85546875" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" style="5" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" customWidth="1"/>
-    <col min="7" max="7" width="2.7109375" customWidth="1"/>
-    <col min="8" max="8" width="6.140625" hidden="1" customWidth="1"/>
-    <col min="9" max="64" width="2.5703125" customWidth="1"/>
-    <col min="69" max="70" width="10.28515625"/>
+    <col min="1" max="1" width="2.6640625" style="58" customWidth="1"/>
+    <col min="2" max="2" width="19.88671875" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" customWidth="1"/>
+    <col min="5" max="5" width="10.44140625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="10.44140625" customWidth="1"/>
+    <col min="7" max="7" width="2.6640625" customWidth="1"/>
+    <col min="8" max="8" width="6.109375" hidden="1" customWidth="1"/>
+    <col min="9" max="64" width="2.5546875" customWidth="1"/>
+    <col min="69" max="70" width="10.33203125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="59" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B1" s="62" t="s">
-        <v>9</v>
+        <v>53</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="2"/>
@@ -1521,44 +1541,46 @@
       <c r="H1" s="2"/>
       <c r="I1" s="85"/>
     </row>
-    <row r="2" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="58" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B2" s="63"/>
       <c r="I2" s="86"/>
     </row>
-    <row r="3" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="58" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B3" s="64" t="s">
-        <v>28</v>
+        <v>54</v>
       </c>
       <c r="C3" s="92" t="s">
         <v>6</v>
       </c>
       <c r="D3" s="93"/>
       <c r="E3" s="91">
-        <f ca="1">TODAY()</f>
-        <v>45069</v>
+        <v>45939</v>
       </c>
       <c r="F3" s="91"/>
     </row>
-    <row r="4" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="59" t="s">
-        <v>38</v>
+        <v>35</v>
+      </c>
+      <c r="B4" s="94" t="s">
+        <v>55</v>
       </c>
       <c r="C4" s="92" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D4" s="93"/>
       <c r="E4" s="7">
         <v>1</v>
       </c>
       <c r="I4" s="88">
-        <f ca="1">I5</f>
-        <v>45068</v>
+        <f>I5</f>
+        <v>45936</v>
       </c>
       <c r="J4" s="89"/>
       <c r="K4" s="89"/>
@@ -1567,8 +1589,8 @@
       <c r="N4" s="89"/>
       <c r="O4" s="90"/>
       <c r="P4" s="88">
-        <f ca="1">P5</f>
-        <v>45075</v>
+        <f>P5</f>
+        <v>45943</v>
       </c>
       <c r="Q4" s="89"/>
       <c r="R4" s="89"/>
@@ -1577,8 +1599,8 @@
       <c r="U4" s="89"/>
       <c r="V4" s="90"/>
       <c r="W4" s="88">
-        <f ca="1">W5</f>
-        <v>45082</v>
+        <f>W5</f>
+        <v>45950</v>
       </c>
       <c r="X4" s="89"/>
       <c r="Y4" s="89"/>
@@ -1587,8 +1609,8 @@
       <c r="AB4" s="89"/>
       <c r="AC4" s="90"/>
       <c r="AD4" s="88">
-        <f ca="1">AD5</f>
-        <v>45089</v>
+        <f>AD5</f>
+        <v>45957</v>
       </c>
       <c r="AE4" s="89"/>
       <c r="AF4" s="89"/>
@@ -1597,8 +1619,8 @@
       <c r="AI4" s="89"/>
       <c r="AJ4" s="90"/>
       <c r="AK4" s="88">
-        <f ca="1">AK5</f>
-        <v>45096</v>
+        <f>AK5</f>
+        <v>45964</v>
       </c>
       <c r="AL4" s="89"/>
       <c r="AM4" s="89"/>
@@ -1607,8 +1629,8 @@
       <c r="AP4" s="89"/>
       <c r="AQ4" s="90"/>
       <c r="AR4" s="88">
-        <f ca="1">AR5</f>
-        <v>45103</v>
+        <f>AR5</f>
+        <v>45971</v>
       </c>
       <c r="AS4" s="89"/>
       <c r="AT4" s="89"/>
@@ -1617,8 +1639,8 @@
       <c r="AW4" s="89"/>
       <c r="AX4" s="90"/>
       <c r="AY4" s="88">
-        <f ca="1">AY5</f>
-        <v>45110</v>
+        <f>AY5</f>
+        <v>45978</v>
       </c>
       <c r="AZ4" s="89"/>
       <c r="BA4" s="89"/>
@@ -1627,8 +1649,8 @@
       <c r="BD4" s="89"/>
       <c r="BE4" s="90"/>
       <c r="BF4" s="88">
-        <f ca="1">BF5</f>
-        <v>45117</v>
+        <f>BF5</f>
+        <v>45985</v>
       </c>
       <c r="BG4" s="89"/>
       <c r="BH4" s="89"/>
@@ -1637,9 +1659,9 @@
       <c r="BK4" s="89"/>
       <c r="BL4" s="90"/>
     </row>
-    <row r="5" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="59" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B5" s="84"/>
       <c r="C5" s="84"/>
@@ -1648,236 +1670,236 @@
       <c r="F5" s="84"/>
       <c r="G5" s="84"/>
       <c r="I5" s="11">
-        <f ca="1">Project_Start-WEEKDAY(Project_Start,1)+2+7*(Display_Week-1)</f>
-        <v>45068</v>
+        <f>Project_Start-WEEKDAY(Project_Start,1)+2+7*(Display_Week-1)</f>
+        <v>45936</v>
       </c>
       <c r="J5" s="10">
-        <f ca="1">I5+1</f>
-        <v>45069</v>
+        <f>I5+1</f>
+        <v>45937</v>
       </c>
       <c r="K5" s="10">
-        <f t="shared" ref="K5:AX5" ca="1" si="0">J5+1</f>
-        <v>45070</v>
+        <f t="shared" ref="K5:AX5" si="0">J5+1</f>
+        <v>45938</v>
       </c>
       <c r="L5" s="10">
-        <f t="shared" ca="1" si="0"/>
-        <v>45071</v>
+        <f t="shared" si="0"/>
+        <v>45939</v>
       </c>
       <c r="M5" s="10">
-        <f t="shared" ca="1" si="0"/>
-        <v>45072</v>
+        <f t="shared" si="0"/>
+        <v>45940</v>
       </c>
       <c r="N5" s="10">
-        <f t="shared" ca="1" si="0"/>
-        <v>45073</v>
+        <f t="shared" si="0"/>
+        <v>45941</v>
       </c>
       <c r="O5" s="12">
-        <f t="shared" ca="1" si="0"/>
-        <v>45074</v>
+        <f t="shared" si="0"/>
+        <v>45942</v>
       </c>
       <c r="P5" s="11">
-        <f ca="1">O5+1</f>
-        <v>45075</v>
+        <f>O5+1</f>
+        <v>45943</v>
       </c>
       <c r="Q5" s="10">
-        <f ca="1">P5+1</f>
-        <v>45076</v>
+        <f>P5+1</f>
+        <v>45944</v>
       </c>
       <c r="R5" s="10">
-        <f t="shared" ca="1" si="0"/>
-        <v>45077</v>
+        <f t="shared" si="0"/>
+        <v>45945</v>
       </c>
       <c r="S5" s="10">
-        <f t="shared" ca="1" si="0"/>
-        <v>45078</v>
+        <f t="shared" si="0"/>
+        <v>45946</v>
       </c>
       <c r="T5" s="10">
-        <f t="shared" ca="1" si="0"/>
-        <v>45079</v>
+        <f t="shared" si="0"/>
+        <v>45947</v>
       </c>
       <c r="U5" s="10">
-        <f t="shared" ca="1" si="0"/>
-        <v>45080</v>
+        <f t="shared" si="0"/>
+        <v>45948</v>
       </c>
       <c r="V5" s="12">
-        <f t="shared" ca="1" si="0"/>
-        <v>45081</v>
+        <f t="shared" si="0"/>
+        <v>45949</v>
       </c>
       <c r="W5" s="11">
-        <f ca="1">V5+1</f>
-        <v>45082</v>
+        <f>V5+1</f>
+        <v>45950</v>
       </c>
       <c r="X5" s="10">
-        <f ca="1">W5+1</f>
-        <v>45083</v>
+        <f>W5+1</f>
+        <v>45951</v>
       </c>
       <c r="Y5" s="10">
-        <f t="shared" ca="1" si="0"/>
-        <v>45084</v>
+        <f t="shared" si="0"/>
+        <v>45952</v>
       </c>
       <c r="Z5" s="10">
-        <f t="shared" ca="1" si="0"/>
-        <v>45085</v>
+        <f t="shared" si="0"/>
+        <v>45953</v>
       </c>
       <c r="AA5" s="10">
-        <f t="shared" ca="1" si="0"/>
-        <v>45086</v>
+        <f t="shared" si="0"/>
+        <v>45954</v>
       </c>
       <c r="AB5" s="10">
-        <f t="shared" ca="1" si="0"/>
-        <v>45087</v>
+        <f t="shared" si="0"/>
+        <v>45955</v>
       </c>
       <c r="AC5" s="12">
-        <f t="shared" ca="1" si="0"/>
-        <v>45088</v>
+        <f t="shared" si="0"/>
+        <v>45956</v>
       </c>
       <c r="AD5" s="11">
-        <f ca="1">AC5+1</f>
-        <v>45089</v>
+        <f>AC5+1</f>
+        <v>45957</v>
       </c>
       <c r="AE5" s="10">
-        <f ca="1">AD5+1</f>
-        <v>45090</v>
+        <f>AD5+1</f>
+        <v>45958</v>
       </c>
       <c r="AF5" s="10">
-        <f t="shared" ca="1" si="0"/>
-        <v>45091</v>
+        <f t="shared" si="0"/>
+        <v>45959</v>
       </c>
       <c r="AG5" s="10">
-        <f t="shared" ca="1" si="0"/>
-        <v>45092</v>
+        <f t="shared" si="0"/>
+        <v>45960</v>
       </c>
       <c r="AH5" s="10">
-        <f t="shared" ca="1" si="0"/>
-        <v>45093</v>
+        <f t="shared" si="0"/>
+        <v>45961</v>
       </c>
       <c r="AI5" s="10">
-        <f t="shared" ca="1" si="0"/>
-        <v>45094</v>
+        <f t="shared" si="0"/>
+        <v>45962</v>
       </c>
       <c r="AJ5" s="12">
-        <f t="shared" ca="1" si="0"/>
-        <v>45095</v>
+        <f t="shared" si="0"/>
+        <v>45963</v>
       </c>
       <c r="AK5" s="11">
-        <f ca="1">AJ5+1</f>
-        <v>45096</v>
+        <f>AJ5+1</f>
+        <v>45964</v>
       </c>
       <c r="AL5" s="10">
-        <f ca="1">AK5+1</f>
-        <v>45097</v>
+        <f>AK5+1</f>
+        <v>45965</v>
       </c>
       <c r="AM5" s="10">
-        <f t="shared" ca="1" si="0"/>
-        <v>45098</v>
+        <f t="shared" si="0"/>
+        <v>45966</v>
       </c>
       <c r="AN5" s="10">
-        <f t="shared" ca="1" si="0"/>
-        <v>45099</v>
+        <f t="shared" si="0"/>
+        <v>45967</v>
       </c>
       <c r="AO5" s="10">
-        <f t="shared" ca="1" si="0"/>
-        <v>45100</v>
+        <f t="shared" si="0"/>
+        <v>45968</v>
       </c>
       <c r="AP5" s="10">
-        <f t="shared" ca="1" si="0"/>
-        <v>45101</v>
+        <f t="shared" si="0"/>
+        <v>45969</v>
       </c>
       <c r="AQ5" s="12">
-        <f t="shared" ca="1" si="0"/>
-        <v>45102</v>
+        <f t="shared" si="0"/>
+        <v>45970</v>
       </c>
       <c r="AR5" s="11">
-        <f ca="1">AQ5+1</f>
-        <v>45103</v>
+        <f>AQ5+1</f>
+        <v>45971</v>
       </c>
       <c r="AS5" s="10">
-        <f ca="1">AR5+1</f>
-        <v>45104</v>
+        <f>AR5+1</f>
+        <v>45972</v>
       </c>
       <c r="AT5" s="10">
-        <f t="shared" ca="1" si="0"/>
-        <v>45105</v>
+        <f t="shared" si="0"/>
+        <v>45973</v>
       </c>
       <c r="AU5" s="10">
-        <f t="shared" ca="1" si="0"/>
-        <v>45106</v>
+        <f t="shared" si="0"/>
+        <v>45974</v>
       </c>
       <c r="AV5" s="10">
-        <f t="shared" ca="1" si="0"/>
-        <v>45107</v>
+        <f t="shared" si="0"/>
+        <v>45975</v>
       </c>
       <c r="AW5" s="10">
-        <f t="shared" ca="1" si="0"/>
-        <v>45108</v>
+        <f t="shared" si="0"/>
+        <v>45976</v>
       </c>
       <c r="AX5" s="12">
-        <f t="shared" ca="1" si="0"/>
-        <v>45109</v>
+        <f t="shared" si="0"/>
+        <v>45977</v>
       </c>
       <c r="AY5" s="11">
-        <f ca="1">AX5+1</f>
-        <v>45110</v>
+        <f>AX5+1</f>
+        <v>45978</v>
       </c>
       <c r="AZ5" s="10">
-        <f ca="1">AY5+1</f>
-        <v>45111</v>
+        <f>AY5+1</f>
+        <v>45979</v>
       </c>
       <c r="BA5" s="10">
-        <f t="shared" ref="BA5:BE5" ca="1" si="1">AZ5+1</f>
-        <v>45112</v>
+        <f t="shared" ref="BA5:BE5" si="1">AZ5+1</f>
+        <v>45980</v>
       </c>
       <c r="BB5" s="10">
-        <f t="shared" ca="1" si="1"/>
-        <v>45113</v>
+        <f t="shared" si="1"/>
+        <v>45981</v>
       </c>
       <c r="BC5" s="10">
-        <f t="shared" ca="1" si="1"/>
-        <v>45114</v>
+        <f t="shared" si="1"/>
+        <v>45982</v>
       </c>
       <c r="BD5" s="10">
-        <f t="shared" ca="1" si="1"/>
-        <v>45115</v>
+        <f t="shared" si="1"/>
+        <v>45983</v>
       </c>
       <c r="BE5" s="12">
-        <f t="shared" ca="1" si="1"/>
-        <v>45116</v>
+        <f t="shared" si="1"/>
+        <v>45984</v>
       </c>
       <c r="BF5" s="11">
-        <f ca="1">BE5+1</f>
-        <v>45117</v>
+        <f>BE5+1</f>
+        <v>45985</v>
       </c>
       <c r="BG5" s="10">
-        <f ca="1">BF5+1</f>
-        <v>45118</v>
+        <f>BF5+1</f>
+        <v>45986</v>
       </c>
       <c r="BH5" s="10">
-        <f t="shared" ref="BH5:BL5" ca="1" si="2">BG5+1</f>
-        <v>45119</v>
+        <f t="shared" ref="BH5:BL5" si="2">BG5+1</f>
+        <v>45987</v>
       </c>
       <c r="BI5" s="10">
-        <f t="shared" ca="1" si="2"/>
-        <v>45120</v>
+        <f t="shared" si="2"/>
+        <v>45988</v>
       </c>
       <c r="BJ5" s="10">
-        <f t="shared" ca="1" si="2"/>
-        <v>45121</v>
+        <f t="shared" si="2"/>
+        <v>45989</v>
       </c>
       <c r="BK5" s="10">
-        <f t="shared" ca="1" si="2"/>
-        <v>45122</v>
+        <f t="shared" si="2"/>
+        <v>45990</v>
       </c>
       <c r="BL5" s="12">
-        <f t="shared" ca="1" si="2"/>
-        <v>45123</v>
-      </c>
-    </row>
-    <row r="6" spans="1:64" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="2"/>
+        <v>45991</v>
+      </c>
+    </row>
+    <row r="6" spans="1:64" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="59" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>8</v>
@@ -1886,243 +1908,243 @@
         <v>7</v>
       </c>
       <c r="E6" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="9" t="s">
         <v>11</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>12</v>
       </c>
       <c r="G6" s="9"/>
       <c r="H6" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I6" s="13" t="str">
-        <f t="shared" ref="I6" ca="1" si="3">LEFT(TEXT(I5,"ddd"),1)</f>
+        <f t="shared" ref="I6" si="3">LEFT(TEXT(I5,"ddd"),1)</f>
         <v>M</v>
       </c>
       <c r="J6" s="13" t="str">
-        <f t="shared" ref="J6:AR6" ca="1" si="4">LEFT(TEXT(J5,"ddd"),1)</f>
+        <f t="shared" ref="J6:AR6" si="4">LEFT(TEXT(J5,"ddd"),1)</f>
         <v>T</v>
       </c>
       <c r="K6" s="13" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" si="4"/>
         <v>W</v>
       </c>
       <c r="L6" s="13" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" si="4"/>
         <v>T</v>
       </c>
       <c r="M6" s="13" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" si="4"/>
         <v>F</v>
       </c>
       <c r="N6" s="13" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" si="4"/>
         <v>S</v>
       </c>
       <c r="O6" s="13" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" si="4"/>
         <v>S</v>
       </c>
       <c r="P6" s="13" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" si="4"/>
         <v>M</v>
       </c>
       <c r="Q6" s="13" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" si="4"/>
         <v>T</v>
       </c>
       <c r="R6" s="13" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" si="4"/>
         <v>W</v>
       </c>
       <c r="S6" s="13" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" si="4"/>
         <v>T</v>
       </c>
       <c r="T6" s="13" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" si="4"/>
         <v>F</v>
       </c>
       <c r="U6" s="13" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" si="4"/>
         <v>S</v>
       </c>
       <c r="V6" s="13" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" si="4"/>
         <v>S</v>
       </c>
       <c r="W6" s="13" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" si="4"/>
         <v>M</v>
       </c>
       <c r="X6" s="13" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" si="4"/>
         <v>T</v>
       </c>
       <c r="Y6" s="13" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" si="4"/>
         <v>W</v>
       </c>
       <c r="Z6" s="13" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" si="4"/>
         <v>T</v>
       </c>
       <c r="AA6" s="13" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" si="4"/>
         <v>F</v>
       </c>
       <c r="AB6" s="13" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" si="4"/>
         <v>S</v>
       </c>
       <c r="AC6" s="13" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" si="4"/>
         <v>S</v>
       </c>
       <c r="AD6" s="13" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" si="4"/>
         <v>M</v>
       </c>
       <c r="AE6" s="13" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" si="4"/>
         <v>T</v>
       </c>
       <c r="AF6" s="13" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" si="4"/>
         <v>W</v>
       </c>
       <c r="AG6" s="13" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" si="4"/>
         <v>T</v>
       </c>
       <c r="AH6" s="13" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" si="4"/>
         <v>F</v>
       </c>
       <c r="AI6" s="13" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" si="4"/>
         <v>S</v>
       </c>
       <c r="AJ6" s="13" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" si="4"/>
         <v>S</v>
       </c>
       <c r="AK6" s="13" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" si="4"/>
         <v>M</v>
       </c>
       <c r="AL6" s="13" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" si="4"/>
         <v>T</v>
       </c>
       <c r="AM6" s="13" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" si="4"/>
         <v>W</v>
       </c>
       <c r="AN6" s="13" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" si="4"/>
         <v>T</v>
       </c>
       <c r="AO6" s="13" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" si="4"/>
         <v>F</v>
       </c>
       <c r="AP6" s="13" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" si="4"/>
         <v>S</v>
       </c>
       <c r="AQ6" s="13" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" si="4"/>
         <v>S</v>
       </c>
       <c r="AR6" s="13" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" si="4"/>
         <v>M</v>
       </c>
       <c r="AS6" s="13" t="str">
-        <f t="shared" ref="AS6:BL6" ca="1" si="5">LEFT(TEXT(AS5,"ddd"),1)</f>
+        <f t="shared" ref="AS6:BL6" si="5">LEFT(TEXT(AS5,"ddd"),1)</f>
         <v>T</v>
       </c>
       <c r="AT6" s="13" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>W</v>
       </c>
       <c r="AU6" s="13" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>T</v>
       </c>
       <c r="AV6" s="13" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>F</v>
       </c>
       <c r="AW6" s="13" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>S</v>
       </c>
       <c r="AX6" s="13" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>S</v>
       </c>
       <c r="AY6" s="13" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>M</v>
       </c>
       <c r="AZ6" s="13" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>T</v>
       </c>
       <c r="BA6" s="13" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>W</v>
       </c>
       <c r="BB6" s="13" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>T</v>
       </c>
       <c r="BC6" s="13" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>F</v>
       </c>
       <c r="BD6" s="13" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>S</v>
       </c>
       <c r="BE6" s="13" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>S</v>
       </c>
       <c r="BF6" s="13" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>M</v>
       </c>
       <c r="BG6" s="13" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>T</v>
       </c>
       <c r="BH6" s="13" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>W</v>
       </c>
       <c r="BI6" s="13" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>T</v>
       </c>
       <c r="BJ6" s="13" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>F</v>
       </c>
       <c r="BK6" s="13" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>S</v>
       </c>
       <c r="BL6" s="13" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>S</v>
       </c>
     </row>
-    <row r="7" spans="1:64" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:64" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="58" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C7" s="61"/>
       <c r="E7"/>
@@ -2187,12 +2209,12 @@
       <c r="BK7" s="44"/>
       <c r="BL7" s="44"/>
     </row>
-    <row r="8" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="59" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C8" s="70"/>
       <c r="D8" s="19"/>
@@ -2260,31 +2282,31 @@
       <c r="BK8" s="44"/>
       <c r="BL8" s="44"/>
     </row>
-    <row r="9" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="59" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B9" s="79" t="s">
-        <v>3</v>
+        <v>48</v>
       </c>
       <c r="C9" s="71" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="D9" s="22">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="E9" s="65">
-        <f ca="1">Project_Start</f>
-        <v>45069</v>
+        <f>Project_Start</f>
+        <v>45939</v>
       </c>
       <c r="F9" s="65">
-        <f ca="1">E9+3</f>
-        <v>45072</v>
+        <f>E9+10</f>
+        <v>45949</v>
       </c>
       <c r="G9" s="17"/>
       <c r="H9" s="17">
-        <f t="shared" ca="1" si="6"/>
-        <v>4</v>
+        <f t="shared" si="6"/>
+        <v>11</v>
       </c>
       <c r="I9" s="44"/>
       <c r="J9" s="44"/>
@@ -2343,29 +2365,31 @@
       <c r="BK9" s="44"/>
       <c r="BL9" s="44"/>
     </row>
-    <row r="10" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="59" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B10" s="79" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" s="71"/>
+        <v>50</v>
+      </c>
+      <c r="C10" s="71" t="s">
+        <v>49</v>
+      </c>
       <c r="D10" s="22">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="E10" s="65">
-        <f ca="1">F9</f>
-        <v>45072</v>
+        <f>F9</f>
+        <v>45949</v>
       </c>
       <c r="F10" s="65">
-        <f ca="1">E10+2</f>
-        <v>45074</v>
+        <f>E10+7</f>
+        <v>45956</v>
       </c>
       <c r="G10" s="17"/>
       <c r="H10" s="17">
-        <f t="shared" ca="1" si="6"/>
-        <v>3</v>
+        <f t="shared" si="6"/>
+        <v>8</v>
       </c>
       <c r="I10" s="44"/>
       <c r="J10" s="44"/>
@@ -2424,19 +2448,29 @@
       <c r="BK10" s="44"/>
       <c r="BL10" s="44"/>
     </row>
-    <row r="11" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="58"/>
       <c r="B11" s="79" t="s">
-        <v>0</v>
-      </c>
-      <c r="C11" s="71"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="65"/>
-      <c r="F11" s="65"/>
+        <v>51</v>
+      </c>
+      <c r="C11" s="71" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" s="22">
+        <v>1</v>
+      </c>
+      <c r="E11" s="65">
+        <f>E10</f>
+        <v>45949</v>
+      </c>
+      <c r="F11" s="65">
+        <f>F10</f>
+        <v>45956</v>
+      </c>
       <c r="G11" s="17"/>
-      <c r="H11" s="17" t="str">
+      <c r="H11" s="17">
         <f t="shared" si="6"/>
-        <v/>
+        <v>8</v>
       </c>
       <c r="I11" s="44"/>
       <c r="J11" s="44"/>
@@ -2495,19 +2529,29 @@
       <c r="BK11" s="44"/>
       <c r="BL11" s="44"/>
     </row>
-    <row r="12" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="58"/>
       <c r="B12" s="79" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" s="71" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" s="22">
         <v>1</v>
       </c>
-      <c r="C12" s="71"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="65"/>
-      <c r="F12" s="65"/>
+      <c r="E12" s="65">
+        <f>E11</f>
+        <v>45949</v>
+      </c>
+      <c r="F12" s="65">
+        <f>F11</f>
+        <v>45956</v>
+      </c>
       <c r="G12" s="17"/>
-      <c r="H12" s="17" t="str">
+      <c r="H12" s="17">
         <f t="shared" si="6"/>
-        <v/>
+        <v>8</v>
       </c>
       <c r="I12" s="44"/>
       <c r="J12" s="44"/>
@@ -2566,7 +2610,7 @@
       <c r="BK12" s="44"/>
       <c r="BL12" s="44"/>
     </row>
-    <row r="13" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="58"/>
       <c r="B13" s="79" t="s">
         <v>2</v>
@@ -2637,12 +2681,12 @@
       <c r="BK13" s="44"/>
       <c r="BL13" s="44"/>
     </row>
-    <row r="14" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="59" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B14" s="23" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C14" s="72"/>
       <c r="D14" s="24"/>
@@ -2710,7 +2754,7 @@
       <c r="BK14" s="44"/>
       <c r="BL14" s="44"/>
     </row>
-    <row r="15" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="59"/>
       <c r="B15" s="80" t="s">
         <v>3</v>
@@ -2781,7 +2825,7 @@
       <c r="BK15" s="44"/>
       <c r="BL15" s="44"/>
     </row>
-    <row r="16" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="58"/>
       <c r="B16" s="80" t="s">
         <v>4</v>
@@ -2852,7 +2896,7 @@
       <c r="BK16" s="44"/>
       <c r="BL16" s="44"/>
     </row>
-    <row r="17" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="58"/>
       <c r="B17" s="80" t="s">
         <v>0</v>
@@ -2923,7 +2967,7 @@
       <c r="BK17" s="44"/>
       <c r="BL17" s="44"/>
     </row>
-    <row r="18" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="58"/>
       <c r="B18" s="80" t="s">
         <v>1</v>
@@ -2994,7 +3038,7 @@
       <c r="BK18" s="44"/>
       <c r="BL18" s="44"/>
     </row>
-    <row r="19" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="58"/>
       <c r="B19" s="80" t="s">
         <v>2</v>
@@ -3065,12 +3109,12 @@
       <c r="BK19" s="44"/>
       <c r="BL19" s="44"/>
     </row>
-    <row r="20" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="58" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B20" s="28" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C20" s="74"/>
       <c r="D20" s="29"/>
@@ -3138,7 +3182,7 @@
       <c r="BK20" s="44"/>
       <c r="BL20" s="44"/>
     </row>
-    <row r="21" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="58"/>
       <c r="B21" s="81" t="s">
         <v>3</v>
@@ -3209,7 +3253,7 @@
       <c r="BK21" s="44"/>
       <c r="BL21" s="44"/>
     </row>
-    <row r="22" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="58"/>
       <c r="B22" s="81" t="s">
         <v>4</v>
@@ -3280,7 +3324,7 @@
       <c r="BK22" s="44"/>
       <c r="BL22" s="44"/>
     </row>
-    <row r="23" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="58"/>
       <c r="B23" s="81" t="s">
         <v>0</v>
@@ -3351,7 +3395,7 @@
       <c r="BK23" s="44"/>
       <c r="BL23" s="44"/>
     </row>
-    <row r="24" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="58"/>
       <c r="B24" s="81"/>
       <c r="C24" s="75"/>
@@ -3417,7 +3461,7 @@
       <c r="BK24" s="44"/>
       <c r="BL24" s="44"/>
     </row>
-    <row r="25" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="58"/>
       <c r="B25" s="81" t="s">
         <v>1</v>
@@ -3488,7 +3532,7 @@
       <c r="BK25" s="44"/>
       <c r="BL25" s="44"/>
     </row>
-    <row r="26" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="58"/>
       <c r="B26" s="81" t="s">
         <v>2</v>
@@ -3559,12 +3603,12 @@
       <c r="BK26" s="44"/>
       <c r="BL26" s="44"/>
     </row>
-    <row r="27" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="58" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B27" s="33" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C27" s="76"/>
       <c r="D27" s="34"/>
@@ -3632,7 +3676,7 @@
       <c r="BK27" s="44"/>
       <c r="BL27" s="44"/>
     </row>
-    <row r="28" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="58"/>
       <c r="B28" s="82" t="s">
         <v>3</v>
@@ -3640,10 +3684,10 @@
       <c r="C28" s="77"/>
       <c r="D28" s="37"/>
       <c r="E28" s="68" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F28" s="68" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G28" s="17"/>
       <c r="H28" s="17" t="e">
@@ -3707,7 +3751,7 @@
       <c r="BK28" s="44"/>
       <c r="BL28" s="44"/>
     </row>
-    <row r="29" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="58"/>
       <c r="B29" s="82" t="s">
         <v>4</v>
@@ -3715,10 +3759,10 @@
       <c r="C29" s="77"/>
       <c r="D29" s="37"/>
       <c r="E29" s="68" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F29" s="68" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G29" s="17"/>
       <c r="H29" s="17" t="e">
@@ -3782,7 +3826,7 @@
       <c r="BK29" s="44"/>
       <c r="BL29" s="44"/>
     </row>
-    <row r="30" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="58"/>
       <c r="B30" s="82" t="s">
         <v>0</v>
@@ -3790,10 +3834,10 @@
       <c r="C30" s="77"/>
       <c r="D30" s="37"/>
       <c r="E30" s="68" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F30" s="68" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G30" s="17"/>
       <c r="H30" s="17" t="e">
@@ -3857,7 +3901,7 @@
       <c r="BK30" s="44"/>
       <c r="BL30" s="44"/>
     </row>
-    <row r="31" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="58"/>
       <c r="B31" s="82" t="s">
         <v>1</v>
@@ -3865,10 +3909,10 @@
       <c r="C31" s="77"/>
       <c r="D31" s="37"/>
       <c r="E31" s="68" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F31" s="68" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G31" s="17"/>
       <c r="H31" s="17" t="e">
@@ -3932,7 +3976,7 @@
       <c r="BK31" s="44"/>
       <c r="BL31" s="44"/>
     </row>
-    <row r="32" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="58"/>
       <c r="B32" s="82" t="s">
         <v>2</v>
@@ -3940,10 +3984,10 @@
       <c r="C32" s="77"/>
       <c r="D32" s="37"/>
       <c r="E32" s="68" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F32" s="68" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G32" s="17"/>
       <c r="H32" s="17" t="e">
@@ -4007,9 +4051,9 @@
       <c r="BK32" s="44"/>
       <c r="BL32" s="44"/>
     </row>
-    <row r="33" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="58" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B33" s="83"/>
       <c r="C33" s="78"/>
@@ -4078,9 +4122,9 @@
       <c r="BK33" s="44"/>
       <c r="BL33" s="44"/>
     </row>
-    <row r="34" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="59" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B34" s="38" t="s">
         <v>5</v>
@@ -4151,14 +4195,14 @@
       <c r="BK34" s="46"/>
       <c r="BL34" s="46"/>
     </row>
-    <row r="35" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G35" s="6"/>
     </row>
-    <row r="36" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C36" s="14"/>
       <c r="F36" s="60"/>
     </row>
-    <row r="37" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C37" s="15"/>
     </row>
   </sheetData>
@@ -4243,88 +4287,88 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="87.140625" style="48" customWidth="1"/>
-    <col min="2" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="87.109375" style="48" customWidth="1"/>
+    <col min="2" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="46.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="1:2" s="50" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="46.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:2" s="50" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="49" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="49"/>
+    </row>
+    <row r="3" spans="1:2" s="54" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="87" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="55"/>
+    </row>
+    <row r="4" spans="1:2" s="51" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
+      <c r="A4" s="52" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="74.099999999999994" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="53" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="52" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" s="48" customFormat="1" ht="204.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="57" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" s="51" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
+      <c r="A8" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="49"/>
-    </row>
-    <row r="3" spans="1:2" s="54" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="87" t="s">
+    </row>
+    <row r="9" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="53" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" s="48" customFormat="1" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="56" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" s="51" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
+      <c r="A11" s="52" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="53" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="55"/>
-    </row>
-    <row r="4" spans="1:2" s="51" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A4" s="52" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="74.099999999999994" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="53" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="52" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" s="48" customFormat="1" ht="204.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="57" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" s="51" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A8" s="52" t="s">
+    </row>
+    <row r="13" spans="1:2" s="48" customFormat="1" ht="27.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="56" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" s="51" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
+      <c r="A14" s="52" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="60" x14ac:dyDescent="0.2">
-      <c r="A9" s="53" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" s="48" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="56" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" s="51" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A11" s="52" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="30" x14ac:dyDescent="0.2">
-      <c r="A12" s="53" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" s="48" customFormat="1" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="56" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" s="51" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A14" s="52" t="s">
+    <row r="15" spans="1:2" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="53" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="53" t="s">
+    <row r="16" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+      <c r="A16" s="53" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="75" x14ac:dyDescent="0.2">
-      <c r="A16" s="53" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -4593,9 +4637,28 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E1A2F4BF-64F9-49C3-913A-DEDB0A7FC48A}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E1A2F4BF-64F9-49C3-913A-DEDB0A7FC48A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="3c7e7f14-e12e-4011-a8f5-4b5c28e9eb09"/>
+    <ds:schemaRef ds:uri="023e2482-3843-4ba8-8468-8ccd9ac81216"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D004AD92-7D8D-4284-9E4A-75773209AD85}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D004AD92-7D8D-4284-9E4A-75773209AD85}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>